<commit_message>
Fixed Current Account Summary
</commit_message>
<xml_diff>
--- a/llm_reconciliation_output.xlsx
+++ b/llm_reconciliation_output.xlsx
@@ -1069,7 +1069,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1100,12 +1100,10 @@
           <t>UNKNOWN DATE</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>299</v>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Generated on 19-Jun-2025 11:10:00 (parsing failed)</t>
+          <t>Unknown (parsing failed)</t>
         </is>
       </c>
     </row>
@@ -1116,11 +1114,11 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>780</v>
+        <v>299</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Amount in Words: 780 Rupees Only (parsing failed)</t>
+          <t>Generated on 19-Jun-2025 11:10:00 (parsing failed)</t>
         </is>
       </c>
     </row>
@@ -1134,6 +1132,21 @@
         <v>780</v>
       </c>
       <c r="C4" t="inlineStr">
+        <is>
+          <t>Amount in Words: 780 Rupees Only (parsing failed)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>UNKNOWN DATE</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>780</v>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>Amount in Words: 780 Rupees Only (parsing failed)</t>
         </is>

</xml_diff>